<commit_message>
feat: -se incorpora seccion k ingreso adultos mayores a pr dependencia
</commit_message>
<xml_diff>
--- a/control_05.xlsx
+++ b/control_05.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pie diabético\Desktop\Main\ESTADISTICAS\SERIES_A\2025\05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90376EFD-97CC-4667-B30C-F5B811F8091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C300B8-A567-4FED-A110-E9245468F443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="202">
   <si>
     <t>MATRONA</t>
   </si>
@@ -1875,6 +1875,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1882,31 +1903,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2793,9 @@
       <c r="D22" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F22" s="100"/>
       <c r="G22" s="99" t="s">
         <v>178</v>
@@ -3112,23 +3114,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="119"/>
       <c r="C1" s="113" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="120" t="s">
         <v>96</v>
       </c>
       <c r="E1" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="F1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="121"/>
+      <c r="G1" s="117"/>
       <c r="H1" s="113" t="s">
         <v>5</v>
       </c>
@@ -3138,10 +3140,10 @@
       <c r="J1" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="119" t="s">
+      <c r="K1" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="117" t="s">
+      <c r="L1" s="111" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3153,7 +3155,7 @@
         <v>108</v>
       </c>
       <c r="C2" s="114"/>
-      <c r="D2" s="116"/>
+      <c r="D2" s="121"/>
       <c r="E2" s="114"/>
       <c r="F2" s="50" t="s">
         <v>100</v>
@@ -3164,8 +3166,8 @@
       <c r="H2" s="114"/>
       <c r="I2" s="114"/>
       <c r="J2" s="114"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="118"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="112"/>
     </row>
     <row r="3" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
@@ -3783,16 +3785,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="J1">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
@@ -3842,10 +3844,10 @@
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="121"/>
+      <c r="C1" s="117"/>
       <c r="D1" s="8" t="s">
         <v>5</v>
       </c>

</xml_diff>